<commit_message>
Put Everything into Functions
But  I will get rid of the hourly chart. I will try to fix the other chart. If I cant fix it, Im just gonna toss it out. I am sure if it is going to be useful.
</commit_message>
<xml_diff>
--- a/Source/Data/reports/MTA_Station_Ridership_Analysis.xlsx
+++ b/Source/Data/reports/MTA_Station_Ridership_Analysis.xlsx
@@ -3937,7 +3937,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>579138</xdr:colOff>
+      <xdr:colOff>582186</xdr:colOff>
       <xdr:row>28</xdr:row>
       <xdr:rowOff>71638</xdr:rowOff>
     </xdr:to>
@@ -3957,7 +3957,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="609600" y="190500"/>
-          <a:ext cx="9113538" cy="5215138"/>
+          <a:ext cx="9116586" cy="5215138"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>

</xml_diff>

<commit_message>
Brought back the version with the other chart version
Its better due to the long station names.
</commit_message>
<xml_diff>
--- a/Source/Data/reports/MTA_Station_Ridership_Analysis.xlsx
+++ b/Source/Data/reports/MTA_Station_Ridership_Analysis.xlsx
@@ -3935,8 +3935,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>201195</xdr:colOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>475510</xdr:colOff>
       <xdr:row>38</xdr:row>
       <xdr:rowOff>163082</xdr:rowOff>
     </xdr:to>
@@ -3956,7 +3956,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="609600" y="190500"/>
-          <a:ext cx="13612395" cy="7211582"/>
+          <a:ext cx="10838710" cy="7211582"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>

</xml_diff>